<commit_message>
Sostituito Partita IVA con Codice Fiscale
</commit_message>
<xml_diff>
--- a/Allegato C - Tracciato xls/TracciatoXLS  - Allegato C.xlsx
+++ b/Allegato C - Tracciato xls/TracciatoXLS  - Allegato C.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iwan/Documents/ARERA/determina_5_ago_2016/Allegato C - Tracciato xls/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE31C41-D460-D345-AC85-8F3FA710F1BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="315" windowWidth="19755" windowHeight="7140"/>
+    <workbookView xWindow="-5120" yWindow="-20520" windowWidth="37660" windowHeight="15360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FlussoTrasporto" sheetId="5" r:id="rId1"/>
@@ -326,18 +332,6 @@
     <t>Corrispettivi</t>
   </si>
   <si>
-    <t>TPartitaIVAMittente</t>
-  </si>
-  <si>
-    <t>Partita IVA del Distributore Mittente</t>
-  </si>
-  <si>
-    <t>TPartitaIVADestinatario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Partita IVA dell'Utente del Trasporto Destinatario </t>
-  </si>
-  <si>
     <t>Numerico (11)</t>
   </si>
   <si>
@@ -783,13 +777,25 @@
   </si>
   <si>
     <t xml:space="preserve">Sezione che contiene il codice del POD </t>
+  </si>
+  <si>
+    <t>TCodFiscaleMittente</t>
+  </si>
+  <si>
+    <t>TCodFiscaleDestinatario</t>
+  </si>
+  <si>
+    <t>Codice Fiscale del Distributore Mittente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Codice Fiscale dell'Utente del Trasporto Destinatario </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1694,6 +1700,162 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1703,55 +1865,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1763,147 +1901,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1950,7 +1964,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1982,9 +1996,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2016,6 +2048,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2191,39 +2241,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24:G30"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="26.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="50.42578125" style="4" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.28515625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="34.28515625" style="4" customWidth="1"/>
-    <col min="18" max="16384" width="12.7109375" style="5"/>
+    <col min="1" max="1" width="19.83203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="13.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="18.83203125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="16.5" style="4" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="26.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="50.5" style="4" customWidth="1"/>
+    <col min="15" max="15" width="10.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.33203125" style="4" customWidth="1"/>
+    <col min="17" max="17" width="34.33203125" style="4" customWidth="1"/>
+    <col min="18" max="16384" width="12.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="37" customFormat="1" ht="24.75" thickBot="1">
+    <row r="1" spans="1:17" s="37" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="39" t="s">
         <v>32</v>
       </c>
@@ -2267,7 +2317,7 @@
         <v>0</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="P1" s="7" t="s">
         <v>2</v>
@@ -2276,120 +2326,120 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="10" customFormat="1">
-      <c r="A2" s="94" t="s">
+    <row r="2" spans="1:17" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A2" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="97" t="s">
-        <v>165</v>
-      </c>
-      <c r="C2" s="100" t="s">
+      <c r="B2" s="111" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="146" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="105" t="s">
+      <c r="D2" s="149" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="137" t="s">
+      <c r="E2" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="133" t="s">
+      <c r="F2" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="135"/>
-      <c r="H2" s="137"/>
-      <c r="I2" s="148"/>
-      <c r="J2" s="135"/>
-      <c r="K2" s="137"/>
-      <c r="L2" s="142"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="94"/>
+      <c r="L2" s="97"/>
       <c r="M2" s="72" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="N2" s="32" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="O2" s="26" t="s">
         <v>3</v>
       </c>
       <c r="P2" s="32" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="Q2" s="33" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" s="10" customFormat="1" ht="24">
-      <c r="A3" s="95"/>
-      <c r="B3" s="98"/>
-      <c r="C3" s="101"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="138"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="136"/>
-      <c r="H3" s="138"/>
-      <c r="I3" s="149"/>
-      <c r="J3" s="136"/>
-      <c r="K3" s="138"/>
-      <c r="L3" s="143"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A3" s="144"/>
+      <c r="B3" s="145"/>
+      <c r="C3" s="147"/>
+      <c r="D3" s="150"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="107"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="98"/>
       <c r="M3" s="54" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="O3" s="16" t="s">
         <v>3</v>
       </c>
       <c r="P3" s="12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="Q3" s="13" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" s="10" customFormat="1">
-      <c r="A4" s="95"/>
-      <c r="B4" s="98"/>
-      <c r="C4" s="101"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="138"/>
-      <c r="F4" s="134"/>
-      <c r="G4" s="136"/>
-      <c r="H4" s="138"/>
-      <c r="I4" s="149"/>
-      <c r="J4" s="136"/>
-      <c r="K4" s="138"/>
-      <c r="L4" s="143"/>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A4" s="144"/>
+      <c r="B4" s="145"/>
+      <c r="C4" s="147"/>
+      <c r="D4" s="150"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="117"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="107"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="95"/>
+      <c r="L4" s="98"/>
       <c r="M4" s="54" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="O4" s="16" t="s">
         <v>3</v>
       </c>
       <c r="P4" s="55" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="Q4" s="13" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" s="10" customFormat="1" ht="24">
-      <c r="A5" s="95"/>
-      <c r="B5" s="98"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="138"/>
-      <c r="F5" s="134"/>
-      <c r="G5" s="136"/>
-      <c r="H5" s="138"/>
-      <c r="I5" s="149"/>
-      <c r="J5" s="136"/>
-      <c r="K5" s="138"/>
-      <c r="L5" s="143"/>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A5" s="144"/>
+      <c r="B5" s="145"/>
+      <c r="C5" s="147"/>
+      <c r="D5" s="150"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="117"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="95"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="95"/>
+      <c r="L5" s="98"/>
       <c r="M5" s="59" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="N5" s="52" t="s">
         <v>40</v>
@@ -2401,24 +2451,24 @@
         <v>35</v>
       </c>
       <c r="Q5" s="13" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" s="10" customFormat="1" ht="24">
-      <c r="A6" s="95"/>
-      <c r="B6" s="98"/>
-      <c r="C6" s="101"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="138"/>
-      <c r="F6" s="134"/>
-      <c r="G6" s="136"/>
-      <c r="H6" s="138"/>
-      <c r="I6" s="149"/>
-      <c r="J6" s="136"/>
-      <c r="K6" s="138"/>
-      <c r="L6" s="143"/>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A6" s="144"/>
+      <c r="B6" s="145"/>
+      <c r="C6" s="147"/>
+      <c r="D6" s="150"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="117"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="95"/>
+      <c r="I6" s="107"/>
+      <c r="J6" s="88"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="98"/>
       <c r="M6" s="54" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="N6" s="55" t="s">
         <v>41</v>
@@ -2430,459 +2480,459 @@
         <v>35</v>
       </c>
       <c r="Q6" s="13" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" s="10" customFormat="1">
-      <c r="A7" s="95"/>
-      <c r="B7" s="98"/>
-      <c r="C7" s="101"/>
-      <c r="D7" s="106"/>
-      <c r="E7" s="138"/>
-      <c r="F7" s="134"/>
-      <c r="G7" s="136"/>
-      <c r="H7" s="138"/>
-      <c r="I7" s="149"/>
-      <c r="J7" s="136"/>
-      <c r="K7" s="138"/>
-      <c r="L7" s="143"/>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A7" s="144"/>
+      <c r="B7" s="145"/>
+      <c r="C7" s="147"/>
+      <c r="D7" s="150"/>
+      <c r="E7" s="95"/>
+      <c r="F7" s="117"/>
+      <c r="G7" s="88"/>
+      <c r="H7" s="95"/>
+      <c r="I7" s="107"/>
+      <c r="J7" s="88"/>
+      <c r="K7" s="95"/>
+      <c r="L7" s="98"/>
       <c r="M7" s="54" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="N7" s="55" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="O7" s="20" t="s">
         <v>3</v>
       </c>
       <c r="P7" s="55" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="Q7" s="56"/>
     </row>
-    <row r="8" spans="1:17" s="10" customFormat="1">
-      <c r="A8" s="95"/>
-      <c r="B8" s="98"/>
-      <c r="C8" s="101"/>
-      <c r="D8" s="106"/>
-      <c r="E8" s="138"/>
-      <c r="F8" s="124"/>
-      <c r="G8" s="120"/>
-      <c r="H8" s="118"/>
-      <c r="I8" s="149"/>
-      <c r="J8" s="120"/>
-      <c r="K8" s="118"/>
-      <c r="L8" s="116"/>
+    <row r="8" spans="1:17" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A8" s="144"/>
+      <c r="B8" s="145"/>
+      <c r="C8" s="147"/>
+      <c r="D8" s="150"/>
+      <c r="E8" s="95"/>
+      <c r="F8" s="92"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="96"/>
+      <c r="I8" s="107"/>
+      <c r="J8" s="85"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="99"/>
       <c r="M8" s="54" t="s">
-        <v>102</v>
+        <v>248</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>103</v>
+        <v>250</v>
       </c>
       <c r="O8" s="16" t="s">
         <v>3</v>
       </c>
       <c r="P8" s="12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="Q8" s="13"/>
     </row>
-    <row r="9" spans="1:17" s="10" customFormat="1">
-      <c r="A9" s="95"/>
-      <c r="B9" s="98"/>
-      <c r="C9" s="101"/>
-      <c r="D9" s="106"/>
-      <c r="E9" s="138"/>
-      <c r="F9" s="124"/>
-      <c r="G9" s="120"/>
-      <c r="H9" s="118"/>
-      <c r="I9" s="149"/>
-      <c r="J9" s="120"/>
-      <c r="K9" s="118"/>
-      <c r="L9" s="116"/>
+    <row r="9" spans="1:17" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A9" s="144"/>
+      <c r="B9" s="145"/>
+      <c r="C9" s="147"/>
+      <c r="D9" s="150"/>
+      <c r="E9" s="95"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="96"/>
+      <c r="I9" s="107"/>
+      <c r="J9" s="85"/>
+      <c r="K9" s="96"/>
+      <c r="L9" s="99"/>
       <c r="M9" s="54" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="N9" s="55" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="O9" s="20" t="s">
         <v>3</v>
       </c>
       <c r="P9" s="55" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="Q9" s="56"/>
     </row>
-    <row r="10" spans="1:17" s="10" customFormat="1">
-      <c r="A10" s="95"/>
-      <c r="B10" s="98"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="106"/>
-      <c r="E10" s="138"/>
-      <c r="F10" s="124"/>
-      <c r="G10" s="120"/>
-      <c r="H10" s="118"/>
-      <c r="I10" s="149"/>
-      <c r="J10" s="120"/>
-      <c r="K10" s="118"/>
-      <c r="L10" s="116"/>
+    <row r="10" spans="1:17" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A10" s="144"/>
+      <c r="B10" s="145"/>
+      <c r="C10" s="147"/>
+      <c r="D10" s="150"/>
+      <c r="E10" s="95"/>
+      <c r="F10" s="92"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="96"/>
+      <c r="I10" s="107"/>
+      <c r="J10" s="85"/>
+      <c r="K10" s="96"/>
+      <c r="L10" s="99"/>
       <c r="M10" s="54" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="N10" s="55" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="O10" s="20" t="s">
         <v>3</v>
       </c>
       <c r="P10" s="55" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="Q10" s="56"/>
     </row>
-    <row r="11" spans="1:17" s="10" customFormat="1">
-      <c r="A11" s="95"/>
-      <c r="B11" s="98"/>
-      <c r="C11" s="101"/>
-      <c r="D11" s="106"/>
-      <c r="E11" s="138"/>
-      <c r="F11" s="124"/>
-      <c r="G11" s="120"/>
-      <c r="H11" s="118"/>
-      <c r="I11" s="149"/>
-      <c r="J11" s="120"/>
-      <c r="K11" s="118"/>
-      <c r="L11" s="116"/>
+    <row r="11" spans="1:17" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A11" s="144"/>
+      <c r="B11" s="145"/>
+      <c r="C11" s="147"/>
+      <c r="D11" s="150"/>
+      <c r="E11" s="95"/>
+      <c r="F11" s="92"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="96"/>
+      <c r="I11" s="107"/>
+      <c r="J11" s="85"/>
+      <c r="K11" s="96"/>
+      <c r="L11" s="99"/>
       <c r="M11" s="54" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="N11" s="55" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="O11" s="20" t="s">
         <v>3</v>
       </c>
       <c r="P11" s="55" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="Q11" s="56"/>
     </row>
-    <row r="12" spans="1:17" s="10" customFormat="1">
-      <c r="A12" s="95"/>
-      <c r="B12" s="98"/>
-      <c r="C12" s="101"/>
-      <c r="D12" s="106"/>
-      <c r="E12" s="138"/>
-      <c r="F12" s="124"/>
-      <c r="G12" s="120"/>
-      <c r="H12" s="118"/>
-      <c r="I12" s="149"/>
-      <c r="J12" s="120"/>
-      <c r="K12" s="118"/>
-      <c r="L12" s="116"/>
+    <row r="12" spans="1:17" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A12" s="144"/>
+      <c r="B12" s="145"/>
+      <c r="C12" s="147"/>
+      <c r="D12" s="150"/>
+      <c r="E12" s="95"/>
+      <c r="F12" s="92"/>
+      <c r="G12" s="85"/>
+      <c r="H12" s="96"/>
+      <c r="I12" s="107"/>
+      <c r="J12" s="85"/>
+      <c r="K12" s="96"/>
+      <c r="L12" s="99"/>
       <c r="M12" s="54" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="N12" s="55" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="O12" s="20" t="s">
         <v>3</v>
       </c>
       <c r="P12" s="55" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="Q12" s="56"/>
     </row>
-    <row r="13" spans="1:17" s="10" customFormat="1">
-      <c r="A13" s="95"/>
-      <c r="B13" s="98"/>
-      <c r="C13" s="101"/>
-      <c r="D13" s="106"/>
-      <c r="E13" s="138"/>
-      <c r="F13" s="124"/>
-      <c r="G13" s="120"/>
-      <c r="H13" s="118"/>
-      <c r="I13" s="149"/>
-      <c r="J13" s="120"/>
-      <c r="K13" s="118"/>
-      <c r="L13" s="116"/>
+    <row r="13" spans="1:17" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A13" s="144"/>
+      <c r="B13" s="145"/>
+      <c r="C13" s="147"/>
+      <c r="D13" s="150"/>
+      <c r="E13" s="95"/>
+      <c r="F13" s="92"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="96"/>
+      <c r="I13" s="107"/>
+      <c r="J13" s="85"/>
+      <c r="K13" s="96"/>
+      <c r="L13" s="99"/>
       <c r="M13" s="54" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="N13" s="55" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="O13" s="20" t="s">
         <v>3</v>
       </c>
       <c r="P13" s="55" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="Q13" s="56"/>
     </row>
-    <row r="14" spans="1:17" s="10" customFormat="1" ht="24">
-      <c r="A14" s="95"/>
-      <c r="B14" s="98"/>
-      <c r="C14" s="101"/>
-      <c r="D14" s="106"/>
-      <c r="E14" s="138"/>
-      <c r="F14" s="124"/>
-      <c r="G14" s="120"/>
-      <c r="H14" s="118"/>
-      <c r="I14" s="149"/>
-      <c r="J14" s="120"/>
-      <c r="K14" s="118"/>
-      <c r="L14" s="116"/>
+    <row r="14" spans="1:17" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A14" s="144"/>
+      <c r="B14" s="145"/>
+      <c r="C14" s="147"/>
+      <c r="D14" s="150"/>
+      <c r="E14" s="95"/>
+      <c r="F14" s="92"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="96"/>
+      <c r="I14" s="107"/>
+      <c r="J14" s="85"/>
+      <c r="K14" s="96"/>
+      <c r="L14" s="99"/>
       <c r="M14" s="54" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="N14" s="55" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="O14" s="20" t="s">
         <v>3</v>
       </c>
       <c r="P14" s="55" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="Q14" s="56"/>
     </row>
-    <row r="15" spans="1:17" s="10" customFormat="1">
-      <c r="A15" s="95"/>
-      <c r="B15" s="98"/>
-      <c r="C15" s="101"/>
-      <c r="D15" s="106"/>
-      <c r="E15" s="138"/>
-      <c r="F15" s="124"/>
-      <c r="G15" s="120"/>
-      <c r="H15" s="118"/>
-      <c r="I15" s="149"/>
-      <c r="J15" s="120"/>
-      <c r="K15" s="118"/>
-      <c r="L15" s="116"/>
+    <row r="15" spans="1:17" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A15" s="144"/>
+      <c r="B15" s="145"/>
+      <c r="C15" s="147"/>
+      <c r="D15" s="150"/>
+      <c r="E15" s="95"/>
+      <c r="F15" s="92"/>
+      <c r="G15" s="85"/>
+      <c r="H15" s="96"/>
+      <c r="I15" s="107"/>
+      <c r="J15" s="85"/>
+      <c r="K15" s="96"/>
+      <c r="L15" s="99"/>
       <c r="M15" s="54" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="N15" s="55" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="O15" s="20" t="s">
         <v>3</v>
       </c>
       <c r="P15" s="55" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="Q15" s="56"/>
     </row>
-    <row r="16" spans="1:17" s="10" customFormat="1">
-      <c r="A16" s="95"/>
-      <c r="B16" s="98"/>
-      <c r="C16" s="101"/>
-      <c r="D16" s="106"/>
-      <c r="E16" s="138"/>
-      <c r="F16" s="124"/>
-      <c r="G16" s="120"/>
-      <c r="H16" s="118"/>
-      <c r="I16" s="149"/>
-      <c r="J16" s="120"/>
-      <c r="K16" s="118"/>
-      <c r="L16" s="116"/>
+    <row r="16" spans="1:17" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A16" s="144"/>
+      <c r="B16" s="145"/>
+      <c r="C16" s="147"/>
+      <c r="D16" s="150"/>
+      <c r="E16" s="95"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="85"/>
+      <c r="H16" s="96"/>
+      <c r="I16" s="107"/>
+      <c r="J16" s="85"/>
+      <c r="K16" s="96"/>
+      <c r="L16" s="99"/>
       <c r="M16" s="54" t="s">
-        <v>104</v>
+        <v>249</v>
       </c>
       <c r="N16" s="12" t="s">
-        <v>105</v>
+        <v>251</v>
       </c>
       <c r="O16" s="16" t="s">
         <v>3</v>
       </c>
       <c r="P16" s="12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="Q16" s="13"/>
     </row>
-    <row r="17" spans="1:17" s="10" customFormat="1">
-      <c r="A17" s="95"/>
-      <c r="B17" s="98"/>
-      <c r="C17" s="101"/>
-      <c r="D17" s="106"/>
-      <c r="E17" s="138"/>
-      <c r="F17" s="124"/>
-      <c r="G17" s="120"/>
-      <c r="H17" s="118"/>
-      <c r="I17" s="149"/>
-      <c r="J17" s="120"/>
-      <c r="K17" s="118"/>
-      <c r="L17" s="116"/>
+    <row r="17" spans="1:17" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A17" s="144"/>
+      <c r="B17" s="145"/>
+      <c r="C17" s="147"/>
+      <c r="D17" s="150"/>
+      <c r="E17" s="95"/>
+      <c r="F17" s="92"/>
+      <c r="G17" s="85"/>
+      <c r="H17" s="96"/>
+      <c r="I17" s="107"/>
+      <c r="J17" s="85"/>
+      <c r="K17" s="96"/>
+      <c r="L17" s="99"/>
       <c r="M17" s="54" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="N17" s="55" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="O17" s="20" t="s">
         <v>3</v>
       </c>
       <c r="P17" s="55" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="Q17" s="56"/>
     </row>
-    <row r="18" spans="1:17" s="10" customFormat="1">
-      <c r="A18" s="95"/>
-      <c r="B18" s="98"/>
-      <c r="C18" s="101"/>
-      <c r="D18" s="106"/>
-      <c r="E18" s="138"/>
-      <c r="F18" s="124"/>
-      <c r="G18" s="120"/>
-      <c r="H18" s="118"/>
-      <c r="I18" s="149"/>
-      <c r="J18" s="120"/>
-      <c r="K18" s="118"/>
-      <c r="L18" s="116"/>
+    <row r="18" spans="1:17" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A18" s="144"/>
+      <c r="B18" s="145"/>
+      <c r="C18" s="147"/>
+      <c r="D18" s="150"/>
+      <c r="E18" s="95"/>
+      <c r="F18" s="92"/>
+      <c r="G18" s="85"/>
+      <c r="H18" s="96"/>
+      <c r="I18" s="107"/>
+      <c r="J18" s="85"/>
+      <c r="K18" s="96"/>
+      <c r="L18" s="99"/>
       <c r="M18" s="54" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="N18" s="55" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="O18" s="20" t="s">
         <v>3</v>
       </c>
       <c r="P18" s="55" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="Q18" s="56"/>
     </row>
-    <row r="19" spans="1:17" s="10" customFormat="1">
-      <c r="A19" s="95"/>
-      <c r="B19" s="98"/>
-      <c r="C19" s="101"/>
-      <c r="D19" s="106"/>
-      <c r="E19" s="138"/>
-      <c r="F19" s="124"/>
-      <c r="G19" s="120"/>
-      <c r="H19" s="118"/>
-      <c r="I19" s="149"/>
-      <c r="J19" s="120"/>
-      <c r="K19" s="118"/>
-      <c r="L19" s="116"/>
+    <row r="19" spans="1:17" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A19" s="144"/>
+      <c r="B19" s="145"/>
+      <c r="C19" s="147"/>
+      <c r="D19" s="150"/>
+      <c r="E19" s="95"/>
+      <c r="F19" s="92"/>
+      <c r="G19" s="85"/>
+      <c r="H19" s="96"/>
+      <c r="I19" s="107"/>
+      <c r="J19" s="85"/>
+      <c r="K19" s="96"/>
+      <c r="L19" s="99"/>
       <c r="M19" s="54" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="N19" s="55" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="O19" s="20" t="s">
         <v>3</v>
       </c>
       <c r="P19" s="55" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="Q19" s="56"/>
     </row>
-    <row r="20" spans="1:17" s="10" customFormat="1">
-      <c r="A20" s="95"/>
-      <c r="B20" s="98"/>
-      <c r="C20" s="101"/>
-      <c r="D20" s="106"/>
-      <c r="E20" s="138"/>
-      <c r="F20" s="124"/>
-      <c r="G20" s="120"/>
-      <c r="H20" s="118"/>
-      <c r="I20" s="149"/>
-      <c r="J20" s="120"/>
-      <c r="K20" s="118"/>
-      <c r="L20" s="116"/>
+    <row r="20" spans="1:17" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A20" s="144"/>
+      <c r="B20" s="145"/>
+      <c r="C20" s="147"/>
+      <c r="D20" s="150"/>
+      <c r="E20" s="95"/>
+      <c r="F20" s="92"/>
+      <c r="G20" s="85"/>
+      <c r="H20" s="96"/>
+      <c r="I20" s="107"/>
+      <c r="J20" s="85"/>
+      <c r="K20" s="96"/>
+      <c r="L20" s="99"/>
       <c r="M20" s="54" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="N20" s="55" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="O20" s="20" t="s">
         <v>3</v>
       </c>
       <c r="P20" s="55" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="Q20" s="56"/>
     </row>
-    <row r="21" spans="1:17" s="10" customFormat="1">
-      <c r="A21" s="95"/>
-      <c r="B21" s="98"/>
-      <c r="C21" s="101"/>
-      <c r="D21" s="106"/>
-      <c r="E21" s="138"/>
-      <c r="F21" s="124"/>
-      <c r="G21" s="120"/>
-      <c r="H21" s="118"/>
-      <c r="I21" s="149"/>
-      <c r="J21" s="120"/>
-      <c r="K21" s="118"/>
-      <c r="L21" s="116"/>
+    <row r="21" spans="1:17" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A21" s="144"/>
+      <c r="B21" s="145"/>
+      <c r="C21" s="147"/>
+      <c r="D21" s="150"/>
+      <c r="E21" s="95"/>
+      <c r="F21" s="92"/>
+      <c r="G21" s="85"/>
+      <c r="H21" s="96"/>
+      <c r="I21" s="107"/>
+      <c r="J21" s="85"/>
+      <c r="K21" s="96"/>
+      <c r="L21" s="99"/>
       <c r="M21" s="54" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="N21" s="55" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="O21" s="20" t="s">
         <v>3</v>
       </c>
       <c r="P21" s="55" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="Q21" s="56"/>
     </row>
-    <row r="22" spans="1:17" s="10" customFormat="1" ht="24.75" thickBot="1">
-      <c r="A22" s="95"/>
-      <c r="B22" s="98"/>
-      <c r="C22" s="101"/>
-      <c r="D22" s="106"/>
-      <c r="E22" s="138"/>
-      <c r="F22" s="124"/>
-      <c r="G22" s="120"/>
-      <c r="H22" s="118"/>
-      <c r="I22" s="149"/>
-      <c r="J22" s="120"/>
-      <c r="K22" s="118"/>
-      <c r="L22" s="116"/>
+    <row r="22" spans="1:17" s="10" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="144"/>
+      <c r="B22" s="145"/>
+      <c r="C22" s="147"/>
+      <c r="D22" s="150"/>
+      <c r="E22" s="95"/>
+      <c r="F22" s="92"/>
+      <c r="G22" s="85"/>
+      <c r="H22" s="96"/>
+      <c r="I22" s="107"/>
+      <c r="J22" s="85"/>
+      <c r="K22" s="96"/>
+      <c r="L22" s="99"/>
       <c r="M22" s="65" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="O22" s="64" t="s">
         <v>3</v>
       </c>
       <c r="P22" s="8" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="Q22" s="63"/>
     </row>
-    <row r="23" spans="1:17" s="10" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A23" s="95"/>
-      <c r="B23" s="98"/>
-      <c r="C23" s="101"/>
-      <c r="D23" s="103" t="s">
-        <v>166</v>
-      </c>
-      <c r="E23" s="97" t="s">
-        <v>172</v>
-      </c>
-      <c r="F23" s="131" t="s">
+    <row r="23" spans="1:17" s="10" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="144"/>
+      <c r="B23" s="145"/>
+      <c r="C23" s="147"/>
+      <c r="D23" s="148" t="s">
+        <v>162</v>
+      </c>
+      <c r="E23" s="111" t="s">
+        <v>168</v>
+      </c>
+      <c r="F23" s="113" t="s">
         <v>3</v>
       </c>
       <c r="G23" s="67" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="H23" s="23" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="I23" s="68" t="s">
         <v>3</v>
@@ -2891,7 +2941,7 @@
       <c r="K23" s="76"/>
       <c r="L23" s="77"/>
       <c r="M23" s="69" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="N23" s="14" t="s">
         <v>39</v>
@@ -2900,116 +2950,116 @@
         <v>3</v>
       </c>
       <c r="P23" s="14" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="Q23" s="25"/>
     </row>
-    <row r="24" spans="1:17" s="1" customFormat="1" ht="24">
-      <c r="A24" s="96"/>
-      <c r="B24" s="99"/>
-      <c r="C24" s="102"/>
-      <c r="D24" s="104"/>
-      <c r="E24" s="99"/>
-      <c r="F24" s="132"/>
-      <c r="G24" s="141" t="s">
-        <v>167</v>
-      </c>
-      <c r="H24" s="118" t="s">
-        <v>230</v>
-      </c>
-      <c r="I24" s="124" t="s">
+    <row r="24" spans="1:17" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A24" s="109"/>
+      <c r="B24" s="112"/>
+      <c r="C24" s="115"/>
+      <c r="D24" s="120"/>
+      <c r="E24" s="112"/>
+      <c r="F24" s="114"/>
+      <c r="G24" s="122" t="s">
+        <v>163</v>
+      </c>
+      <c r="H24" s="96" t="s">
+        <v>226</v>
+      </c>
+      <c r="I24" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="J24" s="120"/>
-      <c r="K24" s="118"/>
-      <c r="L24" s="116"/>
+      <c r="J24" s="85"/>
+      <c r="K24" s="96"/>
+      <c r="L24" s="99"/>
       <c r="M24" s="65" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="O24" s="18" t="s">
         <v>3</v>
       </c>
       <c r="P24" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="Q24" s="62" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="1" customFormat="1" ht="24">
-      <c r="A25" s="96"/>
-      <c r="B25" s="99"/>
-      <c r="C25" s="102"/>
-      <c r="D25" s="104"/>
-      <c r="E25" s="99"/>
-      <c r="F25" s="132"/>
-      <c r="G25" s="120"/>
-      <c r="H25" s="118"/>
-      <c r="I25" s="124"/>
-      <c r="J25" s="120"/>
-      <c r="K25" s="118"/>
-      <c r="L25" s="116"/>
+    <row r="25" spans="1:17" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A25" s="109"/>
+      <c r="B25" s="112"/>
+      <c r="C25" s="115"/>
+      <c r="D25" s="120"/>
+      <c r="E25" s="112"/>
+      <c r="F25" s="114"/>
+      <c r="G25" s="85"/>
+      <c r="H25" s="96"/>
+      <c r="I25" s="92"/>
+      <c r="J25" s="85"/>
+      <c r="K25" s="96"/>
+      <c r="L25" s="99"/>
       <c r="M25" s="65" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="N25" s="8" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="O25" s="18" t="s">
         <v>3</v>
       </c>
       <c r="P25" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="Q25" s="62" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="1" customFormat="1" ht="36">
-      <c r="A26" s="96"/>
-      <c r="B26" s="99"/>
-      <c r="C26" s="102"/>
-      <c r="D26" s="104"/>
-      <c r="E26" s="99"/>
-      <c r="F26" s="132"/>
-      <c r="G26" s="120"/>
-      <c r="H26" s="118"/>
-      <c r="I26" s="124"/>
-      <c r="J26" s="120"/>
-      <c r="K26" s="118"/>
-      <c r="L26" s="116"/>
+    <row r="26" spans="1:17" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A26" s="109"/>
+      <c r="B26" s="112"/>
+      <c r="C26" s="115"/>
+      <c r="D26" s="120"/>
+      <c r="E26" s="112"/>
+      <c r="F26" s="114"/>
+      <c r="G26" s="85"/>
+      <c r="H26" s="96"/>
+      <c r="I26" s="92"/>
+      <c r="J26" s="85"/>
+      <c r="K26" s="96"/>
+      <c r="L26" s="99"/>
       <c r="M26" s="65" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="N26" s="8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="O26" s="18" t="s">
         <v>7</v>
       </c>
       <c r="P26" s="34" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="Q26" s="62" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" s="1" customFormat="1" ht="48">
-      <c r="A27" s="96"/>
-      <c r="B27" s="99"/>
-      <c r="C27" s="102"/>
-      <c r="D27" s="104"/>
-      <c r="E27" s="99"/>
-      <c r="F27" s="132"/>
-      <c r="G27" s="120"/>
-      <c r="H27" s="118"/>
-      <c r="I27" s="124"/>
-      <c r="J27" s="120"/>
-      <c r="K27" s="118"/>
-      <c r="L27" s="116"/>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A27" s="109"/>
+      <c r="B27" s="112"/>
+      <c r="C27" s="115"/>
+      <c r="D27" s="120"/>
+      <c r="E27" s="112"/>
+      <c r="F27" s="114"/>
+      <c r="G27" s="85"/>
+      <c r="H27" s="96"/>
+      <c r="I27" s="92"/>
+      <c r="J27" s="85"/>
+      <c r="K27" s="96"/>
+      <c r="L27" s="99"/>
       <c r="M27" s="54" t="s">
         <v>12</v>
       </c>
@@ -3020,23 +3070,23 @@
         <v>3</v>
       </c>
       <c r="P27" s="55" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="Q27" s="56"/>
     </row>
-    <row r="28" spans="1:17" s="1" customFormat="1" ht="48">
-      <c r="A28" s="96"/>
-      <c r="B28" s="99"/>
-      <c r="C28" s="102"/>
-      <c r="D28" s="104"/>
-      <c r="E28" s="99"/>
-      <c r="F28" s="132"/>
-      <c r="G28" s="120"/>
-      <c r="H28" s="118"/>
-      <c r="I28" s="124"/>
-      <c r="J28" s="120"/>
-      <c r="K28" s="118"/>
-      <c r="L28" s="116"/>
+    <row r="28" spans="1:17" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A28" s="109"/>
+      <c r="B28" s="112"/>
+      <c r="C28" s="115"/>
+      <c r="D28" s="120"/>
+      <c r="E28" s="112"/>
+      <c r="F28" s="114"/>
+      <c r="G28" s="85"/>
+      <c r="H28" s="96"/>
+      <c r="I28" s="92"/>
+      <c r="J28" s="85"/>
+      <c r="K28" s="96"/>
+      <c r="L28" s="99"/>
       <c r="M28" s="54" t="s">
         <v>13</v>
       </c>
@@ -3047,23 +3097,23 @@
         <v>3</v>
       </c>
       <c r="P28" s="55" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="Q28" s="56"/>
     </row>
-    <row r="29" spans="1:17" s="1" customFormat="1" ht="48">
-      <c r="A29" s="96"/>
-      <c r="B29" s="99"/>
-      <c r="C29" s="102"/>
-      <c r="D29" s="104"/>
-      <c r="E29" s="99"/>
-      <c r="F29" s="132"/>
-      <c r="G29" s="120"/>
-      <c r="H29" s="118"/>
-      <c r="I29" s="124"/>
-      <c r="J29" s="120"/>
-      <c r="K29" s="118"/>
-      <c r="L29" s="116"/>
+    <row r="29" spans="1:17" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A29" s="109"/>
+      <c r="B29" s="112"/>
+      <c r="C29" s="115"/>
+      <c r="D29" s="120"/>
+      <c r="E29" s="112"/>
+      <c r="F29" s="114"/>
+      <c r="G29" s="85"/>
+      <c r="H29" s="96"/>
+      <c r="I29" s="92"/>
+      <c r="J29" s="85"/>
+      <c r="K29" s="96"/>
+      <c r="L29" s="99"/>
       <c r="M29" s="54" t="s">
         <v>14</v>
       </c>
@@ -3074,23 +3124,23 @@
         <v>3</v>
       </c>
       <c r="P29" s="55" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="Q29" s="56"/>
     </row>
-    <row r="30" spans="1:17" s="1" customFormat="1" ht="48.75" thickBot="1">
-      <c r="A30" s="96"/>
-      <c r="B30" s="99"/>
-      <c r="C30" s="102"/>
-      <c r="D30" s="104"/>
-      <c r="E30" s="99"/>
-      <c r="F30" s="132"/>
-      <c r="G30" s="121"/>
-      <c r="H30" s="119"/>
-      <c r="I30" s="125"/>
-      <c r="J30" s="121"/>
-      <c r="K30" s="119"/>
-      <c r="L30" s="117"/>
+    <row r="30" spans="1:17" s="1" customFormat="1" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="109"/>
+      <c r="B30" s="112"/>
+      <c r="C30" s="115"/>
+      <c r="D30" s="120"/>
+      <c r="E30" s="112"/>
+      <c r="F30" s="114"/>
+      <c r="G30" s="86"/>
+      <c r="H30" s="118"/>
+      <c r="I30" s="93"/>
+      <c r="J30" s="86"/>
+      <c r="K30" s="118"/>
+      <c r="L30" s="126"/>
       <c r="M30" s="66" t="s">
         <v>15</v>
       </c>
@@ -3101,33 +3151,33 @@
         <v>7</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="Q30" s="3"/>
     </row>
-    <row r="31" spans="1:17" s="1" customFormat="1" ht="48">
-      <c r="A31" s="96"/>
-      <c r="B31" s="99"/>
-      <c r="C31" s="102"/>
-      <c r="D31" s="104"/>
-      <c r="E31" s="99"/>
-      <c r="F31" s="102"/>
-      <c r="G31" s="139" t="s">
+    <row r="31" spans="1:17" s="1" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+      <c r="A31" s="109"/>
+      <c r="B31" s="112"/>
+      <c r="C31" s="115"/>
+      <c r="D31" s="120"/>
+      <c r="E31" s="112"/>
+      <c r="F31" s="115"/>
+      <c r="G31" s="119" t="s">
         <v>36</v>
       </c>
-      <c r="H31" s="110" t="s">
+      <c r="H31" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="I31" s="112" t="s">
+      <c r="I31" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="J31" s="150" t="s">
+      <c r="J31" s="89" t="s">
         <v>76</v>
       </c>
-      <c r="K31" s="110" t="s">
-        <v>170</v>
-      </c>
-      <c r="L31" s="112" t="s">
+      <c r="K31" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="L31" s="103" t="s">
         <v>3</v>
       </c>
       <c r="M31" s="58" t="s">
@@ -3140,25 +3190,25 @@
         <v>7</v>
       </c>
       <c r="P31" s="51" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="Q31" s="81" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" s="1" customFormat="1" ht="36" customHeight="1">
-      <c r="A32" s="96"/>
-      <c r="B32" s="99"/>
-      <c r="C32" s="102"/>
-      <c r="D32" s="104"/>
-      <c r="E32" s="99"/>
-      <c r="F32" s="102"/>
-      <c r="G32" s="104"/>
-      <c r="H32" s="99"/>
-      <c r="I32" s="113"/>
-      <c r="J32" s="151"/>
-      <c r="K32" s="144"/>
-      <c r="L32" s="146"/>
+        <v>246</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="109"/>
+      <c r="B32" s="112"/>
+      <c r="C32" s="115"/>
+      <c r="D32" s="120"/>
+      <c r="E32" s="112"/>
+      <c r="F32" s="115"/>
+      <c r="G32" s="120"/>
+      <c r="H32" s="112"/>
+      <c r="I32" s="123"/>
+      <c r="J32" s="90"/>
+      <c r="K32" s="101"/>
+      <c r="L32" s="104"/>
       <c r="M32" s="54" t="s">
         <v>43</v>
       </c>
@@ -3169,54 +3219,54 @@
         <v>7</v>
       </c>
       <c r="P32" s="55" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="Q32" s="56" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" s="1" customFormat="1" ht="36">
-      <c r="A33" s="96"/>
-      <c r="B33" s="99"/>
-      <c r="C33" s="102"/>
-      <c r="D33" s="104"/>
-      <c r="E33" s="99"/>
-      <c r="F33" s="102"/>
-      <c r="G33" s="104"/>
-      <c r="H33" s="99"/>
-      <c r="I33" s="113"/>
-      <c r="J33" s="151"/>
-      <c r="K33" s="144"/>
-      <c r="L33" s="146"/>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A33" s="109"/>
+      <c r="B33" s="112"/>
+      <c r="C33" s="115"/>
+      <c r="D33" s="120"/>
+      <c r="E33" s="112"/>
+      <c r="F33" s="115"/>
+      <c r="G33" s="120"/>
+      <c r="H33" s="112"/>
+      <c r="I33" s="123"/>
+      <c r="J33" s="90"/>
+      <c r="K33" s="101"/>
+      <c r="L33" s="104"/>
       <c r="M33" s="74" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="N33" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="O33" s="16" t="s">
         <v>7</v>
       </c>
       <c r="P33" s="12" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="Q33" s="13" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" s="1" customFormat="1" ht="24">
-      <c r="A34" s="96"/>
-      <c r="B34" s="99"/>
-      <c r="C34" s="102"/>
-      <c r="D34" s="104"/>
-      <c r="E34" s="99"/>
-      <c r="F34" s="102"/>
-      <c r="G34" s="104"/>
-      <c r="H34" s="99"/>
-      <c r="I34" s="113"/>
-      <c r="J34" s="151"/>
-      <c r="K34" s="144"/>
-      <c r="L34" s="146"/>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A34" s="109"/>
+      <c r="B34" s="112"/>
+      <c r="C34" s="115"/>
+      <c r="D34" s="120"/>
+      <c r="E34" s="112"/>
+      <c r="F34" s="115"/>
+      <c r="G34" s="120"/>
+      <c r="H34" s="112"/>
+      <c r="I34" s="123"/>
+      <c r="J34" s="90"/>
+      <c r="K34" s="101"/>
+      <c r="L34" s="104"/>
       <c r="M34" s="54" t="s">
         <v>44</v>
       </c>
@@ -3227,25 +3277,25 @@
         <v>7</v>
       </c>
       <c r="P34" s="55" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="Q34" s="83" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" s="1" customFormat="1" ht="48">
-      <c r="A35" s="96"/>
-      <c r="B35" s="99"/>
-      <c r="C35" s="102"/>
-      <c r="D35" s="104"/>
-      <c r="E35" s="99"/>
-      <c r="F35" s="102"/>
-      <c r="G35" s="104"/>
-      <c r="H35" s="99"/>
-      <c r="I35" s="113"/>
-      <c r="J35" s="151"/>
-      <c r="K35" s="144"/>
-      <c r="L35" s="146"/>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A35" s="109"/>
+      <c r="B35" s="112"/>
+      <c r="C35" s="115"/>
+      <c r="D35" s="120"/>
+      <c r="E35" s="112"/>
+      <c r="F35" s="115"/>
+      <c r="G35" s="120"/>
+      <c r="H35" s="112"/>
+      <c r="I35" s="123"/>
+      <c r="J35" s="90"/>
+      <c r="K35" s="101"/>
+      <c r="L35" s="104"/>
       <c r="M35" s="54" t="s">
         <v>45</v>
       </c>
@@ -3256,25 +3306,25 @@
         <v>7</v>
       </c>
       <c r="P35" s="55" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="Q35" s="56" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" s="1" customFormat="1" ht="48">
-      <c r="A36" s="96"/>
-      <c r="B36" s="99"/>
-      <c r="C36" s="102"/>
-      <c r="D36" s="104"/>
-      <c r="E36" s="99"/>
-      <c r="F36" s="102"/>
-      <c r="G36" s="104"/>
-      <c r="H36" s="99"/>
-      <c r="I36" s="113"/>
-      <c r="J36" s="151"/>
-      <c r="K36" s="144"/>
-      <c r="L36" s="146"/>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A36" s="109"/>
+      <c r="B36" s="112"/>
+      <c r="C36" s="115"/>
+      <c r="D36" s="120"/>
+      <c r="E36" s="112"/>
+      <c r="F36" s="115"/>
+      <c r="G36" s="120"/>
+      <c r="H36" s="112"/>
+      <c r="I36" s="123"/>
+      <c r="J36" s="90"/>
+      <c r="K36" s="101"/>
+      <c r="L36" s="104"/>
       <c r="M36" s="54" t="s">
         <v>46</v>
       </c>
@@ -3285,25 +3335,25 @@
         <v>7</v>
       </c>
       <c r="P36" s="55" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="Q36" s="56" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" s="1" customFormat="1" ht="48">
-      <c r="A37" s="96"/>
-      <c r="B37" s="99"/>
-      <c r="C37" s="102"/>
-      <c r="D37" s="104"/>
-      <c r="E37" s="99"/>
-      <c r="F37" s="102"/>
-      <c r="G37" s="104"/>
-      <c r="H37" s="99"/>
-      <c r="I37" s="113"/>
-      <c r="J37" s="151"/>
-      <c r="K37" s="144"/>
-      <c r="L37" s="146"/>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A37" s="109"/>
+      <c r="B37" s="112"/>
+      <c r="C37" s="115"/>
+      <c r="D37" s="120"/>
+      <c r="E37" s="112"/>
+      <c r="F37" s="115"/>
+      <c r="G37" s="120"/>
+      <c r="H37" s="112"/>
+      <c r="I37" s="123"/>
+      <c r="J37" s="90"/>
+      <c r="K37" s="101"/>
+      <c r="L37" s="104"/>
       <c r="M37" s="54" t="s">
         <v>47</v>
       </c>
@@ -3314,25 +3364,25 @@
         <v>7</v>
       </c>
       <c r="P37" s="55" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="Q37" s="56" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" s="1" customFormat="1" ht="48">
-      <c r="A38" s="96"/>
-      <c r="B38" s="99"/>
-      <c r="C38" s="102"/>
-      <c r="D38" s="104"/>
-      <c r="E38" s="99"/>
-      <c r="F38" s="102"/>
-      <c r="G38" s="104"/>
-      <c r="H38" s="99"/>
-      <c r="I38" s="113"/>
-      <c r="J38" s="151"/>
-      <c r="K38" s="144"/>
-      <c r="L38" s="146"/>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A38" s="109"/>
+      <c r="B38" s="112"/>
+      <c r="C38" s="115"/>
+      <c r="D38" s="120"/>
+      <c r="E38" s="112"/>
+      <c r="F38" s="115"/>
+      <c r="G38" s="120"/>
+      <c r="H38" s="112"/>
+      <c r="I38" s="123"/>
+      <c r="J38" s="90"/>
+      <c r="K38" s="101"/>
+      <c r="L38" s="104"/>
       <c r="M38" s="54" t="s">
         <v>48</v>
       </c>
@@ -3343,25 +3393,25 @@
         <v>7</v>
       </c>
       <c r="P38" s="55" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="Q38" s="56" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" s="1" customFormat="1" ht="48">
-      <c r="A39" s="96"/>
-      <c r="B39" s="99"/>
-      <c r="C39" s="102"/>
-      <c r="D39" s="104"/>
-      <c r="E39" s="99"/>
-      <c r="F39" s="102"/>
-      <c r="G39" s="104"/>
-      <c r="H39" s="99"/>
-      <c r="I39" s="113"/>
-      <c r="J39" s="151"/>
-      <c r="K39" s="144"/>
-      <c r="L39" s="146"/>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A39" s="109"/>
+      <c r="B39" s="112"/>
+      <c r="C39" s="115"/>
+      <c r="D39" s="120"/>
+      <c r="E39" s="112"/>
+      <c r="F39" s="115"/>
+      <c r="G39" s="120"/>
+      <c r="H39" s="112"/>
+      <c r="I39" s="123"/>
+      <c r="J39" s="90"/>
+      <c r="K39" s="101"/>
+      <c r="L39" s="104"/>
       <c r="M39" s="54" t="s">
         <v>49</v>
       </c>
@@ -3372,25 +3422,25 @@
         <v>7</v>
       </c>
       <c r="P39" s="55" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="Q39" s="56" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" s="1" customFormat="1" ht="48">
-      <c r="A40" s="96"/>
-      <c r="B40" s="99"/>
-      <c r="C40" s="102"/>
-      <c r="D40" s="104"/>
-      <c r="E40" s="99"/>
-      <c r="F40" s="102"/>
-      <c r="G40" s="104"/>
-      <c r="H40" s="99"/>
-      <c r="I40" s="113"/>
-      <c r="J40" s="151"/>
-      <c r="K40" s="144"/>
-      <c r="L40" s="146"/>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A40" s="109"/>
+      <c r="B40" s="112"/>
+      <c r="C40" s="115"/>
+      <c r="D40" s="120"/>
+      <c r="E40" s="112"/>
+      <c r="F40" s="115"/>
+      <c r="G40" s="120"/>
+      <c r="H40" s="112"/>
+      <c r="I40" s="123"/>
+      <c r="J40" s="90"/>
+      <c r="K40" s="101"/>
+      <c r="L40" s="104"/>
       <c r="M40" s="54" t="s">
         <v>50</v>
       </c>
@@ -3401,25 +3451,25 @@
         <v>7</v>
       </c>
       <c r="P40" s="55" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="Q40" s="56" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" s="1" customFormat="1" ht="48">
-      <c r="A41" s="96"/>
-      <c r="B41" s="99"/>
-      <c r="C41" s="102"/>
-      <c r="D41" s="104"/>
-      <c r="E41" s="99"/>
-      <c r="F41" s="102"/>
-      <c r="G41" s="104"/>
-      <c r="H41" s="99"/>
-      <c r="I41" s="113"/>
-      <c r="J41" s="151"/>
-      <c r="K41" s="144"/>
-      <c r="L41" s="146"/>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A41" s="109"/>
+      <c r="B41" s="112"/>
+      <c r="C41" s="115"/>
+      <c r="D41" s="120"/>
+      <c r="E41" s="112"/>
+      <c r="F41" s="115"/>
+      <c r="G41" s="120"/>
+      <c r="H41" s="112"/>
+      <c r="I41" s="123"/>
+      <c r="J41" s="90"/>
+      <c r="K41" s="101"/>
+      <c r="L41" s="104"/>
       <c r="M41" s="54" t="s">
         <v>51</v>
       </c>
@@ -3430,25 +3480,25 @@
         <v>7</v>
       </c>
       <c r="P41" s="55" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="Q41" s="56" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" s="1" customFormat="1" ht="48">
-      <c r="A42" s="96"/>
-      <c r="B42" s="99"/>
-      <c r="C42" s="102"/>
-      <c r="D42" s="104"/>
-      <c r="E42" s="99"/>
-      <c r="F42" s="102"/>
-      <c r="G42" s="104"/>
-      <c r="H42" s="99"/>
-      <c r="I42" s="113"/>
-      <c r="J42" s="151"/>
-      <c r="K42" s="144"/>
-      <c r="L42" s="146"/>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A42" s="109"/>
+      <c r="B42" s="112"/>
+      <c r="C42" s="115"/>
+      <c r="D42" s="120"/>
+      <c r="E42" s="112"/>
+      <c r="F42" s="115"/>
+      <c r="G42" s="120"/>
+      <c r="H42" s="112"/>
+      <c r="I42" s="123"/>
+      <c r="J42" s="90"/>
+      <c r="K42" s="101"/>
+      <c r="L42" s="104"/>
       <c r="M42" s="73" t="s">
         <v>52</v>
       </c>
@@ -3459,25 +3509,25 @@
         <v>7</v>
       </c>
       <c r="P42" s="55" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="Q42" s="56" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" s="1" customFormat="1" ht="48">
-      <c r="A43" s="96"/>
-      <c r="B43" s="99"/>
-      <c r="C43" s="102"/>
-      <c r="D43" s="104"/>
-      <c r="E43" s="99"/>
-      <c r="F43" s="102"/>
-      <c r="G43" s="104"/>
-      <c r="H43" s="99"/>
-      <c r="I43" s="113"/>
-      <c r="J43" s="151"/>
-      <c r="K43" s="144"/>
-      <c r="L43" s="146"/>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A43" s="109"/>
+      <c r="B43" s="112"/>
+      <c r="C43" s="115"/>
+      <c r="D43" s="120"/>
+      <c r="E43" s="112"/>
+      <c r="F43" s="115"/>
+      <c r="G43" s="120"/>
+      <c r="H43" s="112"/>
+      <c r="I43" s="123"/>
+      <c r="J43" s="90"/>
+      <c r="K43" s="101"/>
+      <c r="L43" s="104"/>
       <c r="M43" s="54" t="s">
         <v>53</v>
       </c>
@@ -3488,25 +3538,25 @@
         <v>7</v>
       </c>
       <c r="P43" s="55" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="Q43" s="56" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" s="1" customFormat="1" ht="48">
-      <c r="A44" s="96"/>
-      <c r="B44" s="99"/>
-      <c r="C44" s="102"/>
-      <c r="D44" s="104"/>
-      <c r="E44" s="99"/>
-      <c r="F44" s="102"/>
-      <c r="G44" s="104"/>
-      <c r="H44" s="99"/>
-      <c r="I44" s="113"/>
-      <c r="J44" s="151"/>
-      <c r="K44" s="144"/>
-      <c r="L44" s="146"/>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A44" s="109"/>
+      <c r="B44" s="112"/>
+      <c r="C44" s="115"/>
+      <c r="D44" s="120"/>
+      <c r="E44" s="112"/>
+      <c r="F44" s="115"/>
+      <c r="G44" s="120"/>
+      <c r="H44" s="112"/>
+      <c r="I44" s="123"/>
+      <c r="J44" s="90"/>
+      <c r="K44" s="101"/>
+      <c r="L44" s="104"/>
       <c r="M44" s="54" t="s">
         <v>54</v>
       </c>
@@ -3517,25 +3567,25 @@
         <v>7</v>
       </c>
       <c r="P44" s="55" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="Q44" s="56" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" s="1" customFormat="1" ht="48">
-      <c r="A45" s="96"/>
-      <c r="B45" s="99"/>
-      <c r="C45" s="102"/>
-      <c r="D45" s="104"/>
-      <c r="E45" s="99"/>
-      <c r="F45" s="102"/>
-      <c r="G45" s="104"/>
-      <c r="H45" s="99"/>
-      <c r="I45" s="113"/>
-      <c r="J45" s="151"/>
-      <c r="K45" s="144"/>
-      <c r="L45" s="146"/>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A45" s="109"/>
+      <c r="B45" s="112"/>
+      <c r="C45" s="115"/>
+      <c r="D45" s="120"/>
+      <c r="E45" s="112"/>
+      <c r="F45" s="115"/>
+      <c r="G45" s="120"/>
+      <c r="H45" s="112"/>
+      <c r="I45" s="123"/>
+      <c r="J45" s="90"/>
+      <c r="K45" s="101"/>
+      <c r="L45" s="104"/>
       <c r="M45" s="54" t="s">
         <v>55</v>
       </c>
@@ -3546,25 +3596,25 @@
         <v>7</v>
       </c>
       <c r="P45" s="55" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="Q45" s="56" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" s="1" customFormat="1" ht="48.75" thickBot="1">
-      <c r="A46" s="96"/>
-      <c r="B46" s="99"/>
-      <c r="C46" s="102"/>
-      <c r="D46" s="104"/>
-      <c r="E46" s="99"/>
-      <c r="F46" s="102"/>
-      <c r="G46" s="104"/>
-      <c r="H46" s="99"/>
-      <c r="I46" s="113"/>
-      <c r="J46" s="152"/>
-      <c r="K46" s="145"/>
-      <c r="L46" s="147"/>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" s="1" customFormat="1" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="109"/>
+      <c r="B46" s="112"/>
+      <c r="C46" s="115"/>
+      <c r="D46" s="120"/>
+      <c r="E46" s="112"/>
+      <c r="F46" s="115"/>
+      <c r="G46" s="120"/>
+      <c r="H46" s="112"/>
+      <c r="I46" s="123"/>
+      <c r="J46" s="91"/>
+      <c r="K46" s="102"/>
+      <c r="L46" s="105"/>
       <c r="M46" s="66" t="s">
         <v>56</v>
       </c>
@@ -3575,27 +3625,27 @@
         <v>3</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="Q46" s="3"/>
     </row>
-    <row r="47" spans="1:17" s="1" customFormat="1" ht="36">
-      <c r="A47" s="96"/>
-      <c r="B47" s="99"/>
-      <c r="C47" s="102"/>
-      <c r="D47" s="104"/>
-      <c r="E47" s="99"/>
-      <c r="F47" s="102"/>
-      <c r="G47" s="104"/>
-      <c r="H47" s="99"/>
-      <c r="I47" s="114"/>
-      <c r="J47" s="120" t="s">
+    <row r="47" spans="1:17" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A47" s="109"/>
+      <c r="B47" s="112"/>
+      <c r="C47" s="115"/>
+      <c r="D47" s="120"/>
+      <c r="E47" s="112"/>
+      <c r="F47" s="115"/>
+      <c r="G47" s="120"/>
+      <c r="H47" s="112"/>
+      <c r="I47" s="124"/>
+      <c r="J47" s="85" t="s">
         <v>77</v>
       </c>
-      <c r="K47" s="118" t="s">
-        <v>171</v>
-      </c>
-      <c r="L47" s="108" t="s">
+      <c r="K47" s="96" t="s">
+        <v>167</v>
+      </c>
+      <c r="L47" s="135" t="s">
         <v>3</v>
       </c>
       <c r="M47" s="73" t="s">
@@ -3608,25 +3658,25 @@
         <v>3</v>
       </c>
       <c r="P47" s="38" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="Q47" s="9" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" s="1" customFormat="1" ht="48">
-      <c r="A48" s="96"/>
-      <c r="B48" s="99"/>
-      <c r="C48" s="102"/>
-      <c r="D48" s="104"/>
-      <c r="E48" s="99"/>
-      <c r="F48" s="102"/>
-      <c r="G48" s="104"/>
-      <c r="H48" s="99"/>
-      <c r="I48" s="114"/>
-      <c r="J48" s="120"/>
-      <c r="K48" s="118"/>
-      <c r="L48" s="108"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A48" s="109"/>
+      <c r="B48" s="112"/>
+      <c r="C48" s="115"/>
+      <c r="D48" s="120"/>
+      <c r="E48" s="112"/>
+      <c r="F48" s="115"/>
+      <c r="G48" s="120"/>
+      <c r="H48" s="112"/>
+      <c r="I48" s="124"/>
+      <c r="J48" s="85"/>
+      <c r="K48" s="96"/>
+      <c r="L48" s="135"/>
       <c r="M48" s="54" t="s">
         <v>58</v>
       </c>
@@ -3637,23 +3687,23 @@
         <v>3</v>
       </c>
       <c r="P48" s="55" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="Q48" s="56"/>
     </row>
-    <row r="49" spans="1:17" s="1" customFormat="1" ht="48.75" thickBot="1">
-      <c r="A49" s="96"/>
-      <c r="B49" s="99"/>
-      <c r="C49" s="102"/>
-      <c r="D49" s="104"/>
-      <c r="E49" s="99"/>
-      <c r="F49" s="102"/>
-      <c r="G49" s="104"/>
-      <c r="H49" s="99"/>
-      <c r="I49" s="114"/>
-      <c r="J49" s="121"/>
-      <c r="K49" s="119"/>
-      <c r="L49" s="109"/>
+    <row r="49" spans="1:17" s="1" customFormat="1" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="109"/>
+      <c r="B49" s="112"/>
+      <c r="C49" s="115"/>
+      <c r="D49" s="120"/>
+      <c r="E49" s="112"/>
+      <c r="F49" s="115"/>
+      <c r="G49" s="120"/>
+      <c r="H49" s="112"/>
+      <c r="I49" s="124"/>
+      <c r="J49" s="86"/>
+      <c r="K49" s="118"/>
+      <c r="L49" s="136"/>
       <c r="M49" s="65" t="s">
         <v>59</v>
       </c>
@@ -3664,25 +3714,25 @@
         <v>3</v>
       </c>
       <c r="P49" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="Q49" s="22"/>
     </row>
-    <row r="50" spans="1:17" s="1" customFormat="1" ht="72.75" thickBot="1">
-      <c r="A50" s="96"/>
-      <c r="B50" s="99"/>
-      <c r="C50" s="102"/>
-      <c r="D50" s="104"/>
-      <c r="E50" s="99"/>
-      <c r="F50" s="102"/>
-      <c r="G50" s="140"/>
-      <c r="H50" s="111"/>
-      <c r="I50" s="115"/>
+    <row r="50" spans="1:17" s="1" customFormat="1" ht="66" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="109"/>
+      <c r="B50" s="112"/>
+      <c r="C50" s="115"/>
+      <c r="D50" s="120"/>
+      <c r="E50" s="112"/>
+      <c r="F50" s="115"/>
+      <c r="G50" s="121"/>
+      <c r="H50" s="152"/>
+      <c r="I50" s="125"/>
       <c r="J50" s="70" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="K50" s="57" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="L50" s="71" t="s">
         <v>7</v>
@@ -3691,45 +3741,45 @@
         <v>60</v>
       </c>
       <c r="N50" s="23" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="O50" s="24" t="s">
         <v>7</v>
       </c>
       <c r="P50" s="23" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="Q50" s="25" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" s="1" customFormat="1" ht="36" customHeight="1" thickBot="1">
-      <c r="A51" s="96"/>
-      <c r="B51" s="99"/>
-      <c r="C51" s="102"/>
-      <c r="D51" s="104"/>
-      <c r="E51" s="99"/>
-      <c r="F51" s="132"/>
-      <c r="G51" s="94" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" s="1" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="109"/>
+      <c r="B51" s="112"/>
+      <c r="C51" s="115"/>
+      <c r="D51" s="120"/>
+      <c r="E51" s="112"/>
+      <c r="F51" s="114"/>
+      <c r="G51" s="108" t="s">
         <v>37</v>
       </c>
-      <c r="H51" s="97" t="s">
-        <v>212</v>
-      </c>
-      <c r="I51" s="123" t="s">
+      <c r="H51" s="111" t="s">
+        <v>208</v>
+      </c>
+      <c r="I51" s="128" t="s">
         <v>3</v>
       </c>
       <c r="J51" s="78" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="K51" s="84" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="L51" s="79" t="s">
         <v>3</v>
       </c>
       <c r="M51" s="69" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="N51" s="14" t="s">
         <v>79</v>
@@ -3738,27 +3788,27 @@
         <v>7</v>
       </c>
       <c r="P51" s="14" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="Q51" s="35"/>
     </row>
-    <row r="52" spans="1:17" s="1" customFormat="1" ht="24" customHeight="1">
-      <c r="A52" s="96"/>
-      <c r="B52" s="99"/>
-      <c r="C52" s="102"/>
-      <c r="D52" s="104"/>
-      <c r="E52" s="99"/>
-      <c r="F52" s="132"/>
-      <c r="G52" s="96"/>
-      <c r="H52" s="99"/>
-      <c r="I52" s="124"/>
-      <c r="J52" s="88" t="s">
+    <row r="52" spans="1:17" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="109"/>
+      <c r="B52" s="112"/>
+      <c r="C52" s="115"/>
+      <c r="D52" s="120"/>
+      <c r="E52" s="112"/>
+      <c r="F52" s="114"/>
+      <c r="G52" s="109"/>
+      <c r="H52" s="112"/>
+      <c r="I52" s="92"/>
+      <c r="J52" s="130" t="s">
         <v>97</v>
       </c>
-      <c r="K52" s="91" t="s">
-        <v>225</v>
-      </c>
-      <c r="L52" s="85" t="s">
+      <c r="K52" s="134" t="s">
+        <v>221</v>
+      </c>
+      <c r="L52" s="137" t="s">
         <v>7</v>
       </c>
       <c r="M52" s="73" t="s">
@@ -3771,25 +3821,25 @@
         <v>7</v>
       </c>
       <c r="P52" s="55" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="Q52" s="9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" s="1" customFormat="1" ht="36">
-      <c r="A53" s="96"/>
-      <c r="B53" s="99"/>
-      <c r="C53" s="102"/>
-      <c r="D53" s="104"/>
-      <c r="E53" s="99"/>
-      <c r="F53" s="132"/>
-      <c r="G53" s="96"/>
-      <c r="H53" s="99"/>
-      <c r="I53" s="124"/>
-      <c r="J53" s="89"/>
-      <c r="K53" s="92"/>
-      <c r="L53" s="86"/>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A53" s="109"/>
+      <c r="B53" s="112"/>
+      <c r="C53" s="115"/>
+      <c r="D53" s="120"/>
+      <c r="E53" s="112"/>
+      <c r="F53" s="114"/>
+      <c r="G53" s="109"/>
+      <c r="H53" s="112"/>
+      <c r="I53" s="92"/>
+      <c r="J53" s="140"/>
+      <c r="K53" s="142"/>
+      <c r="L53" s="138"/>
       <c r="M53" s="54" t="s">
         <v>62</v>
       </c>
@@ -3800,23 +3850,23 @@
         <v>7</v>
       </c>
       <c r="P53" s="55" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="Q53" s="56"/>
     </row>
-    <row r="54" spans="1:17" s="1" customFormat="1" ht="36">
-      <c r="A54" s="96"/>
-      <c r="B54" s="99"/>
-      <c r="C54" s="102"/>
-      <c r="D54" s="104"/>
-      <c r="E54" s="99"/>
-      <c r="F54" s="132"/>
-      <c r="G54" s="96"/>
-      <c r="H54" s="99"/>
-      <c r="I54" s="124"/>
-      <c r="J54" s="89"/>
-      <c r="K54" s="92"/>
-      <c r="L54" s="86"/>
+    <row r="54" spans="1:17" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A54" s="109"/>
+      <c r="B54" s="112"/>
+      <c r="C54" s="115"/>
+      <c r="D54" s="120"/>
+      <c r="E54" s="112"/>
+      <c r="F54" s="114"/>
+      <c r="G54" s="109"/>
+      <c r="H54" s="112"/>
+      <c r="I54" s="92"/>
+      <c r="J54" s="140"/>
+      <c r="K54" s="142"/>
+      <c r="L54" s="138"/>
       <c r="M54" s="54" t="s">
         <v>63</v>
       </c>
@@ -3827,23 +3877,23 @@
         <v>7</v>
       </c>
       <c r="P54" s="55" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="Q54" s="56"/>
     </row>
-    <row r="55" spans="1:17" s="1" customFormat="1" ht="36">
-      <c r="A55" s="96"/>
-      <c r="B55" s="99"/>
-      <c r="C55" s="102"/>
-      <c r="D55" s="104"/>
-      <c r="E55" s="99"/>
-      <c r="F55" s="132"/>
-      <c r="G55" s="96"/>
-      <c r="H55" s="99"/>
-      <c r="I55" s="124"/>
-      <c r="J55" s="89"/>
-      <c r="K55" s="92"/>
-      <c r="L55" s="86"/>
+    <row r="55" spans="1:17" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A55" s="109"/>
+      <c r="B55" s="112"/>
+      <c r="C55" s="115"/>
+      <c r="D55" s="120"/>
+      <c r="E55" s="112"/>
+      <c r="F55" s="114"/>
+      <c r="G55" s="109"/>
+      <c r="H55" s="112"/>
+      <c r="I55" s="92"/>
+      <c r="J55" s="140"/>
+      <c r="K55" s="142"/>
+      <c r="L55" s="138"/>
       <c r="M55" s="54" t="s">
         <v>64</v>
       </c>
@@ -3854,25 +3904,25 @@
         <v>7</v>
       </c>
       <c r="P55" s="55" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="Q55" s="56" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" s="1" customFormat="1" ht="36">
-      <c r="A56" s="96"/>
-      <c r="B56" s="99"/>
-      <c r="C56" s="102"/>
-      <c r="D56" s="104"/>
-      <c r="E56" s="99"/>
-      <c r="F56" s="132"/>
-      <c r="G56" s="96"/>
-      <c r="H56" s="99"/>
-      <c r="I56" s="124"/>
-      <c r="J56" s="89"/>
-      <c r="K56" s="92"/>
-      <c r="L56" s="86"/>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A56" s="109"/>
+      <c r="B56" s="112"/>
+      <c r="C56" s="115"/>
+      <c r="D56" s="120"/>
+      <c r="E56" s="112"/>
+      <c r="F56" s="114"/>
+      <c r="G56" s="109"/>
+      <c r="H56" s="112"/>
+      <c r="I56" s="92"/>
+      <c r="J56" s="140"/>
+      <c r="K56" s="142"/>
+      <c r="L56" s="138"/>
       <c r="M56" s="54" t="s">
         <v>65</v>
       </c>
@@ -3883,25 +3933,25 @@
         <v>7</v>
       </c>
       <c r="P56" s="55" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="Q56" s="56" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" s="1" customFormat="1" ht="24">
-      <c r="A57" s="96"/>
-      <c r="B57" s="99"/>
-      <c r="C57" s="102"/>
-      <c r="D57" s="104"/>
-      <c r="E57" s="99"/>
-      <c r="F57" s="132"/>
-      <c r="G57" s="96"/>
-      <c r="H57" s="99"/>
-      <c r="I57" s="124"/>
-      <c r="J57" s="89"/>
-      <c r="K57" s="92"/>
-      <c r="L57" s="86"/>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A57" s="109"/>
+      <c r="B57" s="112"/>
+      <c r="C57" s="115"/>
+      <c r="D57" s="120"/>
+      <c r="E57" s="112"/>
+      <c r="F57" s="114"/>
+      <c r="G57" s="109"/>
+      <c r="H57" s="112"/>
+      <c r="I57" s="92"/>
+      <c r="J57" s="140"/>
+      <c r="K57" s="142"/>
+      <c r="L57" s="138"/>
       <c r="M57" s="54" t="s">
         <v>66</v>
       </c>
@@ -3912,25 +3962,25 @@
         <v>7</v>
       </c>
       <c r="P57" s="55" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="Q57" s="56" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" s="1" customFormat="1" ht="24">
-      <c r="A58" s="96"/>
-      <c r="B58" s="99"/>
-      <c r="C58" s="102"/>
-      <c r="D58" s="104"/>
-      <c r="E58" s="99"/>
-      <c r="F58" s="132"/>
-      <c r="G58" s="96"/>
-      <c r="H58" s="99"/>
-      <c r="I58" s="124"/>
-      <c r="J58" s="89"/>
-      <c r="K58" s="92"/>
-      <c r="L58" s="86"/>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A58" s="109"/>
+      <c r="B58" s="112"/>
+      <c r="C58" s="115"/>
+      <c r="D58" s="120"/>
+      <c r="E58" s="112"/>
+      <c r="F58" s="114"/>
+      <c r="G58" s="109"/>
+      <c r="H58" s="112"/>
+      <c r="I58" s="92"/>
+      <c r="J58" s="140"/>
+      <c r="K58" s="142"/>
+      <c r="L58" s="138"/>
       <c r="M58" s="54" t="s">
         <v>67</v>
       </c>
@@ -3941,205 +3991,205 @@
         <v>7</v>
       </c>
       <c r="P58" s="55" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="Q58" s="56" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" s="1" customFormat="1" ht="24">
-      <c r="A59" s="96"/>
-      <c r="B59" s="99"/>
-      <c r="C59" s="102"/>
-      <c r="D59" s="104"/>
-      <c r="E59" s="99"/>
-      <c r="F59" s="132"/>
-      <c r="G59" s="96"/>
-      <c r="H59" s="99"/>
-      <c r="I59" s="124"/>
-      <c r="J59" s="89"/>
-      <c r="K59" s="92"/>
-      <c r="L59" s="86"/>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A59" s="109"/>
+      <c r="B59" s="112"/>
+      <c r="C59" s="115"/>
+      <c r="D59" s="120"/>
+      <c r="E59" s="112"/>
+      <c r="F59" s="114"/>
+      <c r="G59" s="109"/>
+      <c r="H59" s="112"/>
+      <c r="I59" s="92"/>
+      <c r="J59" s="140"/>
+      <c r="K59" s="142"/>
+      <c r="L59" s="138"/>
       <c r="M59" s="54" t="s">
         <v>68</v>
       </c>
       <c r="N59" s="55" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="O59" s="20" t="s">
         <v>7</v>
       </c>
       <c r="P59" s="55" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="Q59" s="56" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" s="1" customFormat="1" ht="48.75" thickBot="1">
-      <c r="A60" s="96"/>
-      <c r="B60" s="99"/>
-      <c r="C60" s="102"/>
-      <c r="D60" s="104"/>
-      <c r="E60" s="99"/>
-      <c r="F60" s="132"/>
-      <c r="G60" s="96"/>
-      <c r="H60" s="99"/>
-      <c r="I60" s="124"/>
-      <c r="J60" s="90"/>
-      <c r="K60" s="93"/>
-      <c r="L60" s="87"/>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" s="1" customFormat="1" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="109"/>
+      <c r="B60" s="112"/>
+      <c r="C60" s="115"/>
+      <c r="D60" s="120"/>
+      <c r="E60" s="112"/>
+      <c r="F60" s="114"/>
+      <c r="G60" s="109"/>
+      <c r="H60" s="112"/>
+      <c r="I60" s="92"/>
+      <c r="J60" s="141"/>
+      <c r="K60" s="143"/>
+      <c r="L60" s="139"/>
       <c r="M60" s="65" t="s">
         <v>69</v>
       </c>
       <c r="N60" s="60" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="O60" s="27" t="s">
         <v>7</v>
       </c>
       <c r="P60" s="60" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="Q60" s="62" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" s="1" customFormat="1" ht="36">
-      <c r="A61" s="96"/>
-      <c r="B61" s="99"/>
-      <c r="C61" s="102"/>
-      <c r="D61" s="104"/>
-      <c r="E61" s="99"/>
-      <c r="F61" s="132"/>
-      <c r="G61" s="96"/>
-      <c r="H61" s="99"/>
-      <c r="I61" s="124"/>
-      <c r="J61" s="126" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A61" s="109"/>
+      <c r="B61" s="112"/>
+      <c r="C61" s="115"/>
+      <c r="D61" s="120"/>
+      <c r="E61" s="112"/>
+      <c r="F61" s="114"/>
+      <c r="G61" s="109"/>
+      <c r="H61" s="112"/>
+      <c r="I61" s="92"/>
+      <c r="J61" s="129" t="s">
         <v>101</v>
       </c>
-      <c r="K61" s="129" t="s">
-        <v>173</v>
-      </c>
-      <c r="L61" s="107" t="s">
+      <c r="K61" s="133" t="s">
+        <v>169</v>
+      </c>
+      <c r="L61" s="151" t="s">
         <v>7</v>
       </c>
       <c r="M61" s="53" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="N61" s="28" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="O61" s="29" t="s">
         <v>7</v>
       </c>
       <c r="P61" s="28" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="Q61" s="30" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" s="1" customFormat="1" ht="36">
-      <c r="A62" s="96"/>
-      <c r="B62" s="99"/>
-      <c r="C62" s="102"/>
-      <c r="D62" s="104"/>
-      <c r="E62" s="99"/>
-      <c r="F62" s="132"/>
-      <c r="G62" s="96"/>
-      <c r="H62" s="99"/>
-      <c r="I62" s="124"/>
-      <c r="J62" s="88"/>
-      <c r="K62" s="91"/>
-      <c r="L62" s="85"/>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A62" s="109"/>
+      <c r="B62" s="112"/>
+      <c r="C62" s="115"/>
+      <c r="D62" s="120"/>
+      <c r="E62" s="112"/>
+      <c r="F62" s="114"/>
+      <c r="G62" s="109"/>
+      <c r="H62" s="112"/>
+      <c r="I62" s="92"/>
+      <c r="J62" s="130"/>
+      <c r="K62" s="134"/>
+      <c r="L62" s="137"/>
       <c r="M62" s="73" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="N62" s="31" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="O62" s="17" t="s">
         <v>7</v>
       </c>
       <c r="P62" s="31" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="Q62" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" s="1" customFormat="1" ht="60">
-      <c r="A63" s="96"/>
-      <c r="B63" s="99"/>
-      <c r="C63" s="102"/>
-      <c r="D63" s="104"/>
-      <c r="E63" s="99"/>
-      <c r="F63" s="132"/>
-      <c r="G63" s="96"/>
-      <c r="H63" s="99"/>
-      <c r="I63" s="124"/>
-      <c r="J63" s="88"/>
-      <c r="K63" s="91"/>
-      <c r="L63" s="85"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" s="1" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+      <c r="A63" s="109"/>
+      <c r="B63" s="112"/>
+      <c r="C63" s="115"/>
+      <c r="D63" s="120"/>
+      <c r="E63" s="112"/>
+      <c r="F63" s="114"/>
+      <c r="G63" s="109"/>
+      <c r="H63" s="112"/>
+      <c r="I63" s="92"/>
+      <c r="J63" s="130"/>
+      <c r="K63" s="134"/>
+      <c r="L63" s="137"/>
       <c r="M63" s="73" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="N63" s="31" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="O63" s="17" t="s">
         <v>7</v>
       </c>
       <c r="P63" s="31" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="Q63" s="11" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" s="1" customFormat="1" ht="24">
-      <c r="A64" s="96"/>
-      <c r="B64" s="99"/>
-      <c r="C64" s="102"/>
-      <c r="D64" s="104"/>
-      <c r="E64" s="99"/>
-      <c r="F64" s="132"/>
-      <c r="G64" s="96"/>
-      <c r="H64" s="99"/>
-      <c r="I64" s="124"/>
-      <c r="J64" s="88"/>
-      <c r="K64" s="91"/>
-      <c r="L64" s="85"/>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A64" s="109"/>
+      <c r="B64" s="112"/>
+      <c r="C64" s="115"/>
+      <c r="D64" s="120"/>
+      <c r="E64" s="112"/>
+      <c r="F64" s="114"/>
+      <c r="G64" s="109"/>
+      <c r="H64" s="112"/>
+      <c r="I64" s="92"/>
+      <c r="J64" s="130"/>
+      <c r="K64" s="134"/>
+      <c r="L64" s="137"/>
       <c r="M64" s="73" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="N64" s="31" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="O64" s="17" t="s">
         <v>7</v>
       </c>
       <c r="P64" s="31" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="Q64" s="11" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" s="1" customFormat="1" ht="36">
-      <c r="A65" s="96"/>
-      <c r="B65" s="99"/>
-      <c r="C65" s="102"/>
-      <c r="D65" s="104"/>
-      <c r="E65" s="99"/>
-      <c r="F65" s="132"/>
-      <c r="G65" s="96"/>
-      <c r="H65" s="99"/>
-      <c r="I65" s="124"/>
-      <c r="J65" s="127"/>
-      <c r="K65" s="118"/>
-      <c r="L65" s="108"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A65" s="109"/>
+      <c r="B65" s="112"/>
+      <c r="C65" s="115"/>
+      <c r="D65" s="120"/>
+      <c r="E65" s="112"/>
+      <c r="F65" s="114"/>
+      <c r="G65" s="109"/>
+      <c r="H65" s="112"/>
+      <c r="I65" s="92"/>
+      <c r="J65" s="131"/>
+      <c r="K65" s="96"/>
+      <c r="L65" s="135"/>
       <c r="M65" s="73" t="s">
         <v>70</v>
       </c>
@@ -4150,52 +4200,52 @@
         <v>7</v>
       </c>
       <c r="P65" s="38" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="Q65" s="9" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="66" spans="1:17" s="1" customFormat="1" ht="12" customHeight="1">
-      <c r="A66" s="96"/>
-      <c r="B66" s="99"/>
-      <c r="C66" s="102"/>
-      <c r="D66" s="104"/>
-      <c r="E66" s="99"/>
-      <c r="F66" s="132"/>
-      <c r="G66" s="96"/>
-      <c r="H66" s="99"/>
-      <c r="I66" s="124"/>
-      <c r="J66" s="127"/>
-      <c r="K66" s="118"/>
-      <c r="L66" s="108"/>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="109"/>
+      <c r="B66" s="112"/>
+      <c r="C66" s="115"/>
+      <c r="D66" s="120"/>
+      <c r="E66" s="112"/>
+      <c r="F66" s="114"/>
+      <c r="G66" s="109"/>
+      <c r="H66" s="112"/>
+      <c r="I66" s="92"/>
+      <c r="J66" s="131"/>
+      <c r="K66" s="96"/>
+      <c r="L66" s="135"/>
       <c r="M66" s="73" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="N66" s="38" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="O66" s="21" t="s">
         <v>7</v>
       </c>
       <c r="P66" s="55" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="Q66" s="9"/>
     </row>
-    <row r="67" spans="1:17" s="1" customFormat="1" ht="24">
-      <c r="A67" s="96"/>
-      <c r="B67" s="99"/>
-      <c r="C67" s="102"/>
-      <c r="D67" s="104"/>
-      <c r="E67" s="99"/>
-      <c r="F67" s="132"/>
-      <c r="G67" s="96"/>
-      <c r="H67" s="99"/>
-      <c r="I67" s="124"/>
-      <c r="J67" s="127"/>
-      <c r="K67" s="118"/>
-      <c r="L67" s="108"/>
+    <row r="67" spans="1:17" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A67" s="109"/>
+      <c r="B67" s="112"/>
+      <c r="C67" s="115"/>
+      <c r="D67" s="120"/>
+      <c r="E67" s="112"/>
+      <c r="F67" s="114"/>
+      <c r="G67" s="109"/>
+      <c r="H67" s="112"/>
+      <c r="I67" s="92"/>
+      <c r="J67" s="131"/>
+      <c r="K67" s="96"/>
+      <c r="L67" s="135"/>
       <c r="M67" s="54" t="s">
         <v>71</v>
       </c>
@@ -4206,25 +4256,25 @@
         <v>3</v>
       </c>
       <c r="P67" s="55" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="Q67" s="56" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" s="1" customFormat="1" ht="24">
-      <c r="A68" s="96"/>
-      <c r="B68" s="99"/>
-      <c r="C68" s="102"/>
-      <c r="D68" s="104"/>
-      <c r="E68" s="99"/>
-      <c r="F68" s="132"/>
-      <c r="G68" s="96"/>
-      <c r="H68" s="99"/>
-      <c r="I68" s="124"/>
-      <c r="J68" s="127"/>
-      <c r="K68" s="118"/>
-      <c r="L68" s="108"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A68" s="109"/>
+      <c r="B68" s="112"/>
+      <c r="C68" s="115"/>
+      <c r="D68" s="120"/>
+      <c r="E68" s="112"/>
+      <c r="F68" s="114"/>
+      <c r="G68" s="109"/>
+      <c r="H68" s="112"/>
+      <c r="I68" s="92"/>
+      <c r="J68" s="131"/>
+      <c r="K68" s="96"/>
+      <c r="L68" s="135"/>
       <c r="M68" s="54" t="s">
         <v>72</v>
       </c>
@@ -4238,22 +4288,22 @@
         <v>35</v>
       </c>
       <c r="Q68" s="56" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17" s="1" customFormat="1" ht="24">
-      <c r="A69" s="96"/>
-      <c r="B69" s="99"/>
-      <c r="C69" s="102"/>
-      <c r="D69" s="104"/>
-      <c r="E69" s="99"/>
-      <c r="F69" s="132"/>
-      <c r="G69" s="96"/>
-      <c r="H69" s="99"/>
-      <c r="I69" s="124"/>
-      <c r="J69" s="127"/>
-      <c r="K69" s="118"/>
-      <c r="L69" s="108"/>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A69" s="109"/>
+      <c r="B69" s="112"/>
+      <c r="C69" s="115"/>
+      <c r="D69" s="120"/>
+      <c r="E69" s="112"/>
+      <c r="F69" s="114"/>
+      <c r="G69" s="109"/>
+      <c r="H69" s="112"/>
+      <c r="I69" s="92"/>
+      <c r="J69" s="131"/>
+      <c r="K69" s="96"/>
+      <c r="L69" s="135"/>
       <c r="M69" s="54" t="s">
         <v>73</v>
       </c>
@@ -4267,196 +4317,196 @@
         <v>35</v>
       </c>
       <c r="Q69" s="56" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="70" spans="1:17" s="1" customFormat="1" ht="24">
-      <c r="A70" s="96"/>
-      <c r="B70" s="99"/>
-      <c r="C70" s="102"/>
-      <c r="D70" s="104"/>
-      <c r="E70" s="99"/>
-      <c r="F70" s="132"/>
-      <c r="G70" s="96"/>
-      <c r="H70" s="99"/>
-      <c r="I70" s="124"/>
-      <c r="J70" s="127"/>
-      <c r="K70" s="118"/>
-      <c r="L70" s="108"/>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A70" s="109"/>
+      <c r="B70" s="112"/>
+      <c r="C70" s="115"/>
+      <c r="D70" s="120"/>
+      <c r="E70" s="112"/>
+      <c r="F70" s="114"/>
+      <c r="G70" s="109"/>
+      <c r="H70" s="112"/>
+      <c r="I70" s="92"/>
+      <c r="J70" s="131"/>
+      <c r="K70" s="96"/>
+      <c r="L70" s="135"/>
       <c r="M70" s="54" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N70" s="55" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="O70" s="20" t="s">
         <v>7</v>
       </c>
       <c r="P70" s="55" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="Q70" s="56" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17" s="1" customFormat="1" ht="48">
-      <c r="A71" s="96"/>
-      <c r="B71" s="99"/>
-      <c r="C71" s="102"/>
-      <c r="D71" s="104"/>
-      <c r="E71" s="99"/>
-      <c r="F71" s="132"/>
-      <c r="G71" s="96"/>
-      <c r="H71" s="99"/>
-      <c r="I71" s="124"/>
-      <c r="J71" s="127"/>
-      <c r="K71" s="118"/>
-      <c r="L71" s="108"/>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" s="1" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+      <c r="A71" s="109"/>
+      <c r="B71" s="112"/>
+      <c r="C71" s="115"/>
+      <c r="D71" s="120"/>
+      <c r="E71" s="112"/>
+      <c r="F71" s="114"/>
+      <c r="G71" s="109"/>
+      <c r="H71" s="112"/>
+      <c r="I71" s="92"/>
+      <c r="J71" s="131"/>
+      <c r="K71" s="96"/>
+      <c r="L71" s="135"/>
       <c r="M71" s="54" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="N71" s="55" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="O71" s="20" t="s">
         <v>7</v>
       </c>
       <c r="P71" s="55" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="Q71" s="56" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" s="1" customFormat="1" ht="48">
-      <c r="A72" s="96"/>
-      <c r="B72" s="99"/>
-      <c r="C72" s="102"/>
-      <c r="D72" s="104"/>
-      <c r="E72" s="99"/>
-      <c r="F72" s="132"/>
-      <c r="G72" s="96"/>
-      <c r="H72" s="99"/>
-      <c r="I72" s="124"/>
-      <c r="J72" s="127"/>
-      <c r="K72" s="118"/>
-      <c r="L72" s="108"/>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A72" s="109"/>
+      <c r="B72" s="112"/>
+      <c r="C72" s="115"/>
+      <c r="D72" s="120"/>
+      <c r="E72" s="112"/>
+      <c r="F72" s="114"/>
+      <c r="G72" s="109"/>
+      <c r="H72" s="112"/>
+      <c r="I72" s="92"/>
+      <c r="J72" s="131"/>
+      <c r="K72" s="96"/>
+      <c r="L72" s="135"/>
       <c r="M72" s="54" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="N72" s="55" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="O72" s="20" t="s">
         <v>7</v>
       </c>
       <c r="P72" s="55" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="Q72" s="56" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" s="1" customFormat="1" ht="48">
-      <c r="A73" s="96"/>
-      <c r="B73" s="99"/>
-      <c r="C73" s="102"/>
-      <c r="D73" s="104"/>
-      <c r="E73" s="99"/>
-      <c r="F73" s="132"/>
-      <c r="G73" s="96"/>
-      <c r="H73" s="99"/>
-      <c r="I73" s="124"/>
-      <c r="J73" s="127"/>
-      <c r="K73" s="118"/>
-      <c r="L73" s="108"/>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A73" s="109"/>
+      <c r="B73" s="112"/>
+      <c r="C73" s="115"/>
+      <c r="D73" s="120"/>
+      <c r="E73" s="112"/>
+      <c r="F73" s="114"/>
+      <c r="G73" s="109"/>
+      <c r="H73" s="112"/>
+      <c r="I73" s="92"/>
+      <c r="J73" s="131"/>
+      <c r="K73" s="96"/>
+      <c r="L73" s="135"/>
       <c r="M73" s="54" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="N73" s="55" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="O73" s="20" t="s">
         <v>7</v>
       </c>
       <c r="P73" s="55" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q73" s="56" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="109"/>
+      <c r="B74" s="112"/>
+      <c r="C74" s="115"/>
+      <c r="D74" s="120"/>
+      <c r="E74" s="112"/>
+      <c r="F74" s="114"/>
+      <c r="G74" s="109"/>
+      <c r="H74" s="112"/>
+      <c r="I74" s="92"/>
+      <c r="J74" s="131"/>
+      <c r="K74" s="96"/>
+      <c r="L74" s="135"/>
+      <c r="M74" s="54" t="s">
         <v>124</v>
       </c>
-      <c r="Q73" s="56" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="74" spans="1:17" s="1" customFormat="1" ht="12" customHeight="1">
-      <c r="A74" s="96"/>
-      <c r="B74" s="99"/>
-      <c r="C74" s="102"/>
-      <c r="D74" s="104"/>
-      <c r="E74" s="99"/>
-      <c r="F74" s="132"/>
-      <c r="G74" s="96"/>
-      <c r="H74" s="99"/>
-      <c r="I74" s="124"/>
-      <c r="J74" s="127"/>
-      <c r="K74" s="118"/>
-      <c r="L74" s="108"/>
-      <c r="M74" s="54" t="s">
-        <v>128</v>
-      </c>
       <c r="N74" s="55" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="O74" s="20" t="s">
         <v>7</v>
       </c>
       <c r="P74" s="55" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="Q74" s="56" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="75" spans="1:17" s="1" customFormat="1" ht="48">
-      <c r="A75" s="96"/>
-      <c r="B75" s="99"/>
-      <c r="C75" s="102"/>
-      <c r="D75" s="104"/>
-      <c r="E75" s="99"/>
-      <c r="F75" s="132"/>
-      <c r="G75" s="96"/>
-      <c r="H75" s="99"/>
-      <c r="I75" s="124"/>
-      <c r="J75" s="127"/>
-      <c r="K75" s="118"/>
-      <c r="L75" s="108"/>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A75" s="109"/>
+      <c r="B75" s="112"/>
+      <c r="C75" s="115"/>
+      <c r="D75" s="120"/>
+      <c r="E75" s="112"/>
+      <c r="F75" s="114"/>
+      <c r="G75" s="109"/>
+      <c r="H75" s="112"/>
+      <c r="I75" s="92"/>
+      <c r="J75" s="131"/>
+      <c r="K75" s="96"/>
+      <c r="L75" s="135"/>
       <c r="M75" s="54" t="s">
         <v>74</v>
       </c>
       <c r="N75" s="55" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="O75" s="20" t="s">
         <v>7</v>
       </c>
       <c r="P75" s="55" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="Q75" s="56" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="76" spans="1:17" s="1" customFormat="1" ht="48">
-      <c r="A76" s="96"/>
-      <c r="B76" s="99"/>
-      <c r="C76" s="102"/>
-      <c r="D76" s="104"/>
-      <c r="E76" s="99"/>
-      <c r="F76" s="132"/>
-      <c r="G76" s="96"/>
-      <c r="H76" s="99"/>
-      <c r="I76" s="124"/>
-      <c r="J76" s="127"/>
-      <c r="K76" s="118"/>
-      <c r="L76" s="108"/>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A76" s="109"/>
+      <c r="B76" s="112"/>
+      <c r="C76" s="115"/>
+      <c r="D76" s="120"/>
+      <c r="E76" s="112"/>
+      <c r="F76" s="114"/>
+      <c r="G76" s="109"/>
+      <c r="H76" s="112"/>
+      <c r="I76" s="92"/>
+      <c r="J76" s="131"/>
+      <c r="K76" s="96"/>
+      <c r="L76" s="135"/>
       <c r="M76" s="74" t="s">
         <v>98</v>
       </c>
@@ -4467,25 +4517,25 @@
         <v>7</v>
       </c>
       <c r="P76" s="12" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="Q76" s="62" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="77" spans="1:17" s="1" customFormat="1" ht="12" customHeight="1">
-      <c r="A77" s="96"/>
-      <c r="B77" s="99"/>
-      <c r="C77" s="102"/>
-      <c r="D77" s="104"/>
-      <c r="E77" s="99"/>
-      <c r="F77" s="132"/>
-      <c r="G77" s="96"/>
-      <c r="H77" s="99"/>
-      <c r="I77" s="124"/>
-      <c r="J77" s="127"/>
-      <c r="K77" s="118"/>
-      <c r="L77" s="108"/>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="109"/>
+      <c r="B77" s="112"/>
+      <c r="C77" s="115"/>
+      <c r="D77" s="120"/>
+      <c r="E77" s="112"/>
+      <c r="F77" s="114"/>
+      <c r="G77" s="109"/>
+      <c r="H77" s="112"/>
+      <c r="I77" s="92"/>
+      <c r="J77" s="131"/>
+      <c r="K77" s="96"/>
+      <c r="L77" s="135"/>
       <c r="M77" s="54" t="s">
         <v>99</v>
       </c>
@@ -4496,25 +4546,25 @@
         <v>3</v>
       </c>
       <c r="P77" s="55" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="Q77" s="13" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="78" spans="1:17" s="1" customFormat="1" ht="48.75" thickBot="1">
-      <c r="A78" s="96"/>
-      <c r="B78" s="99"/>
-      <c r="C78" s="102"/>
-      <c r="D78" s="104"/>
-      <c r="E78" s="99"/>
-      <c r="F78" s="132"/>
-      <c r="G78" s="130"/>
-      <c r="H78" s="122"/>
-      <c r="I78" s="125"/>
-      <c r="J78" s="128"/>
-      <c r="K78" s="119"/>
-      <c r="L78" s="109"/>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" s="1" customFormat="1" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="109"/>
+      <c r="B78" s="112"/>
+      <c r="C78" s="115"/>
+      <c r="D78" s="120"/>
+      <c r="E78" s="112"/>
+      <c r="F78" s="114"/>
+      <c r="G78" s="110"/>
+      <c r="H78" s="127"/>
+      <c r="I78" s="93"/>
+      <c r="J78" s="132"/>
+      <c r="K78" s="118"/>
+      <c r="L78" s="136"/>
       <c r="M78" s="66" t="s">
         <v>100</v>
       </c>
@@ -4525,11 +4575,11 @@
         <v>3</v>
       </c>
       <c r="P78" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="Q78" s="3"/>
     </row>
-    <row r="79" spans="1:17">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" s="5"/>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
@@ -4543,7 +4593,7 @@
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
     </row>
-    <row r="80" spans="1:17">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" s="5"/>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
@@ -4557,7 +4607,7 @@
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
     </row>
-    <row r="81" spans="1:12">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" s="5"/>
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
@@ -4573,16 +4623,11 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="J47:J49"/>
-    <mergeCell ref="J2:J22"/>
-    <mergeCell ref="J31:J46"/>
-    <mergeCell ref="I24:I30"/>
-    <mergeCell ref="K2:K22"/>
-    <mergeCell ref="L2:L22"/>
-    <mergeCell ref="K31:K46"/>
-    <mergeCell ref="L31:L46"/>
-    <mergeCell ref="I2:I22"/>
-    <mergeCell ref="G51:G78"/>
+    <mergeCell ref="A2:A78"/>
+    <mergeCell ref="B2:B78"/>
+    <mergeCell ref="C2:C78"/>
+    <mergeCell ref="D23:D78"/>
+    <mergeCell ref="D2:D22"/>
     <mergeCell ref="E23:E78"/>
     <mergeCell ref="F23:F78"/>
     <mergeCell ref="F2:F22"/>
@@ -4593,25 +4638,30 @@
     <mergeCell ref="G24:G30"/>
     <mergeCell ref="H2:H22"/>
     <mergeCell ref="I31:I50"/>
-    <mergeCell ref="L24:L30"/>
     <mergeCell ref="K24:K30"/>
     <mergeCell ref="J24:J30"/>
     <mergeCell ref="H51:H78"/>
     <mergeCell ref="I51:I78"/>
     <mergeCell ref="J61:J78"/>
     <mergeCell ref="K61:K78"/>
+    <mergeCell ref="L2:L22"/>
+    <mergeCell ref="K31:K46"/>
+    <mergeCell ref="L31:L46"/>
+    <mergeCell ref="I2:I22"/>
+    <mergeCell ref="G51:G78"/>
+    <mergeCell ref="L24:L30"/>
     <mergeCell ref="L47:L49"/>
     <mergeCell ref="H24:H30"/>
     <mergeCell ref="L52:L60"/>
     <mergeCell ref="J52:J60"/>
     <mergeCell ref="K52:K60"/>
-    <mergeCell ref="A2:A78"/>
-    <mergeCell ref="B2:B78"/>
-    <mergeCell ref="C2:C78"/>
-    <mergeCell ref="D23:D78"/>
-    <mergeCell ref="D2:D22"/>
     <mergeCell ref="L61:L78"/>
     <mergeCell ref="H31:H50"/>
+    <mergeCell ref="J47:J49"/>
+    <mergeCell ref="J2:J22"/>
+    <mergeCell ref="J31:J46"/>
+    <mergeCell ref="I24:I30"/>
+    <mergeCell ref="K2:K22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>